<commit_message>
Change the logic of goods search key
</commit_message>
<xml_diff>
--- a/platform/service-boss/src/main/resources/download/good_search_key.xlsx
+++ b/platform/service-boss/src/main/resources/download/good_search_key.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fgh\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fgh\IdeaProjects\mall-shop\platform\service-boss\src\main\resources\download\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65F2A087-19CB-4405-9AAD-FE55E8F7176E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D29A443-211A-4C43-8550-FCB4CC6988BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12144" yWindow="1320" windowWidth="20028" windowHeight="11580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="60" yWindow="660" windowWidth="20028" windowHeight="11580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,16 +25,32 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>关键字</t>
   </si>
   <si>
-    <t>spu_id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>商品名称</t>
+    <t>绑定商品名称</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>绑定商品SPU_ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>关联商品SPU_ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>关联商品SKU_ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>链接</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>类型(1商品,2链接)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -360,23 +376,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.88671875" customWidth="1"/>
+    <col min="5" max="6" width="16.109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>